<commit_message>
1.  Initialised spreadsheets after cmip5 initialisation file specified.
</commit_message>
<xml_diff>
--- a/cmip6/models/cnrm-cm6-1/cmip6_cnrm-cerfacs_cnrm-cm6-1_toplevel.xlsx
+++ b/cmip6/models/cnrm-cm6-1/cmip6_cnrm-cerfacs_cnrm-cm6-1_toplevel.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="784" uniqueCount="418">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="786" uniqueCount="420">
   <si>
     <t>ES-DOC CMIP6 Model Documentation</t>
   </si>
@@ -139,6 +139,9 @@
     <t>cmip6.toplevel.key_properties.name</t>
   </si>
   <si>
+    <t>CNRM-CM5</t>
+  </si>
+  <si>
     <t>1.1.1.2 *</t>
   </si>
   <si>
@@ -167,6 +170,9 @@
   </si>
   <si>
     <t>NOTE: Double click to expand if text is too long for cell</t>
+  </si>
+  <si>
+    <t>As the coastlines in the ocean and in the atmosphere models do not match, global operations are used to force the absolute conservation of fluxes or a redistribution of the fluxes proportional to the respective ocean and atmosphere basin surfaces (see details in Valcke 2012)</t>
   </si>
   <si>
     <t>1.2.1</t>
@@ -2019,14 +2025,16 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="24" customHeight="1">
-      <c r="B6" s="11"/>
+      <c r="B6" s="11" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="8" spans="1:3" ht="24" customHeight="1">
       <c r="A8" s="9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="24" customHeight="1">
@@ -2034,15 +2042,15 @@
         <v>37</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="24" customHeight="1">
       <c r="B10" s="8" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="24" customHeight="1">
@@ -2050,10 +2058,10 @@
     </row>
     <row r="13" spans="1:3" ht="24" customHeight="1">
       <c r="A13" s="9" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="24" customHeight="1">
@@ -2061,39 +2069,41 @@
         <v>37</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="24" customHeight="1">
       <c r="B15" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="178" customHeight="1">
-      <c r="B16" s="11"/>
+      <c r="B16" s="11" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="19" spans="1:3" ht="24" customHeight="1">
       <c r="A19" s="12" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="24" customHeight="1">
       <c r="B20" s="13" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="24" customHeight="1">
       <c r="A22" s="9" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="24" customHeight="1">
@@ -2101,15 +2111,15 @@
         <v>37</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="24" customHeight="1">
       <c r="B24" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="178" customHeight="1">
@@ -2117,23 +2127,23 @@
     </row>
     <row r="28" spans="1:3" ht="24" customHeight="1">
       <c r="A28" s="12" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="24" customHeight="1">
       <c r="B29" s="13" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="24" customHeight="1">
       <c r="A31" s="9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="24" customHeight="1">
@@ -2141,10 +2151,10 @@
         <v>37</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="24" customHeight="1">
@@ -2152,10 +2162,10 @@
     </row>
     <row r="35" spans="1:3" ht="24" customHeight="1">
       <c r="A35" s="9" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="24" customHeight="1">
@@ -2163,10 +2173,10 @@
         <v>37</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="24" customHeight="1">
@@ -2174,10 +2184,10 @@
     </row>
     <row r="39" spans="1:3" ht="24" customHeight="1">
       <c r="A39" s="9" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="24" customHeight="1">
@@ -2185,10 +2195,10 @@
         <v>37</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C40" s="10" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="24" customHeight="1">
@@ -2196,10 +2206,10 @@
     </row>
     <row r="43" spans="1:3" ht="24" customHeight="1">
       <c r="A43" s="9" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="24" customHeight="1">
@@ -2207,15 +2217,15 @@
         <v>37</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C44" s="10" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="24" customHeight="1">
       <c r="B45" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="178" customHeight="1">
@@ -2223,10 +2233,10 @@
     </row>
     <row r="48" spans="1:3" ht="24" customHeight="1">
       <c r="A48" s="9" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="24" customHeight="1">
@@ -2234,10 +2244,10 @@
         <v>37</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C49" s="10" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="24" customHeight="1">
@@ -2245,23 +2255,23 @@
     </row>
     <row r="53" spans="1:3" ht="24" customHeight="1">
       <c r="A53" s="12" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B53" s="12" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="24" customHeight="1">
       <c r="B54" s="13" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="24" customHeight="1">
       <c r="A56" s="9" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B56" s="9" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="24" customHeight="1">
@@ -2269,10 +2279,10 @@
         <v>37</v>
       </c>
       <c r="B57" s="10" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C57" s="10" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="24" customHeight="1">
@@ -2280,10 +2290,10 @@
     </row>
     <row r="60" spans="1:3" ht="24" customHeight="1">
       <c r="A60" s="9" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B60" s="9" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="24" customHeight="1">
@@ -2291,10 +2301,10 @@
         <v>37</v>
       </c>
       <c r="B61" s="10" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C61" s="10" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="24" customHeight="1">
@@ -2302,10 +2312,10 @@
     </row>
     <row r="64" spans="1:3" ht="24" customHeight="1">
       <c r="A64" s="9" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B64" s="9" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="65" spans="1:34" ht="24" customHeight="1">
@@ -2313,15 +2323,15 @@
         <v>37</v>
       </c>
       <c r="B65" s="10" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C65" s="10" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="66" spans="1:34" ht="24" customHeight="1">
       <c r="B66" s="8" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="67" spans="1:34" ht="24" customHeight="1">
@@ -2329,10 +2339,10 @@
     </row>
     <row r="69" spans="1:34" ht="24" customHeight="1">
       <c r="A69" s="9" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B69" s="9" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="70" spans="1:34" ht="24" customHeight="1">
@@ -2340,10 +2350,10 @@
         <v>37</v>
       </c>
       <c r="B70" s="10" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C70" s="10" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="71" spans="1:34" ht="24" customHeight="1">
@@ -2351,56 +2361,56 @@
     </row>
     <row r="73" spans="1:34" ht="24" customHeight="1">
       <c r="A73" s="9" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B73" s="9" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="74" spans="1:34" ht="24" customHeight="1">
       <c r="A74" s="14" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B74" s="10" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C74" s="10" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="75" spans="1:34" ht="24" customHeight="1">
       <c r="B75" s="11"/>
       <c r="AA75" s="6" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="AB75" s="6" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="AC75" s="6" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="AD75" s="6" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="AE75" s="6" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="AF75" s="6" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="AG75" s="6" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="AH75" s="6" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="78" spans="1:34" ht="24" customHeight="1">
       <c r="A78" s="12" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B78" s="12" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="79" spans="1:34" ht="24" customHeight="1">
@@ -2408,21 +2418,21 @@
     </row>
     <row r="81" spans="1:30" ht="24" customHeight="1">
       <c r="A81" s="9" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B81" s="9" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="82" spans="1:30" ht="24" customHeight="1">
       <c r="A82" s="14" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B82" s="10" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="C82" s="10" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="83" spans="1:30" ht="24" customHeight="1">
@@ -2430,55 +2440,55 @@
     </row>
     <row r="85" spans="1:30" ht="24" customHeight="1">
       <c r="A85" s="9" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B85" s="9" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="86" spans="1:30" ht="24" customHeight="1">
       <c r="A86" s="14" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B86" s="10" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C86" s="10" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="87" spans="1:30" ht="24" customHeight="1">
       <c r="B87" s="11"/>
       <c r="AA87" s="6" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="AB87" s="6" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="AC87" s="6" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="AD87" s="6" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="89" spans="1:30" ht="24" customHeight="1">
       <c r="A89" s="9" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B89" s="9" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="90" spans="1:30" ht="24" customHeight="1">
       <c r="A90" s="14" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B90" s="10" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C90" s="10" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="91" spans="1:30" ht="24" customHeight="1">
@@ -2486,23 +2496,23 @@
     </row>
     <row r="94" spans="1:30" ht="24" customHeight="1">
       <c r="A94" s="12" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B94" s="12" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
     </row>
     <row r="95" spans="1:30" ht="24" customHeight="1">
       <c r="B95" s="13" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="24" customHeight="1">
       <c r="A97" s="9" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B97" s="9" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="24" customHeight="1">
@@ -2510,15 +2520,15 @@
         <v>37</v>
       </c>
       <c r="B98" s="10" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C98" s="10" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
     <row r="99" spans="1:3" ht="24" customHeight="1">
       <c r="B99" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="178" customHeight="1">
@@ -2526,10 +2536,10 @@
     </row>
     <row r="102" spans="1:3" ht="24" customHeight="1">
       <c r="A102" s="9" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B102" s="9" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="103" spans="1:3" ht="24" customHeight="1">
@@ -2537,15 +2547,15 @@
         <v>37</v>
       </c>
       <c r="B103" s="10" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C103" s="10" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="24" customHeight="1">
       <c r="B104" s="8" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="24" customHeight="1">
@@ -2553,10 +2563,10 @@
     </row>
     <row r="107" spans="1:3" ht="24" customHeight="1">
       <c r="A107" s="9" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B107" s="9" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
     <row r="108" spans="1:3" ht="24" customHeight="1">
@@ -2564,15 +2574,15 @@
         <v>37</v>
       </c>
       <c r="B108" s="10" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="C108" s="10" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="109" spans="1:3" ht="24" customHeight="1">
       <c r="B109" s="8" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="110" spans="1:3" ht="24" customHeight="1">
@@ -2580,10 +2590,10 @@
     </row>
     <row r="112" spans="1:3" ht="24" customHeight="1">
       <c r="A112" s="9" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B112" s="9" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row r="113" spans="1:3" ht="24" customHeight="1">
@@ -2591,15 +2601,15 @@
         <v>37</v>
       </c>
       <c r="B113" s="10" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="C113" s="10" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="114" spans="1:3" ht="24" customHeight="1">
       <c r="B114" s="8" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="115" spans="1:3" ht="24" customHeight="1">
@@ -2607,10 +2617,10 @@
     </row>
     <row r="117" spans="1:3" ht="24" customHeight="1">
       <c r="A117" s="9" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B117" s="9" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="118" spans="1:3" ht="24" customHeight="1">
@@ -2618,10 +2628,10 @@
         <v>37</v>
       </c>
       <c r="B118" s="10" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="C118" s="10" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="119" spans="1:3" ht="24" customHeight="1">
@@ -2629,10 +2639,10 @@
     </row>
     <row r="121" spans="1:3" ht="24" customHeight="1">
       <c r="A121" s="9" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B121" s="9" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="122" spans="1:3" ht="24" customHeight="1">
@@ -2640,10 +2650,10 @@
         <v>37</v>
       </c>
       <c r="B122" s="10" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="C122" s="10" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="123" spans="1:3" ht="24" customHeight="1">
@@ -2651,23 +2661,23 @@
     </row>
     <row r="126" spans="1:3" ht="24" customHeight="1">
       <c r="A126" s="12" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B126" s="12" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row r="127" spans="1:3" ht="24" customHeight="1">
       <c r="B127" s="13" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
     </row>
     <row r="129" spans="1:3" ht="24" customHeight="1">
       <c r="A129" s="9" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="B129" s="9" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
     </row>
     <row r="130" spans="1:3" ht="24" customHeight="1">
@@ -2675,15 +2685,15 @@
         <v>37</v>
       </c>
       <c r="B130" s="10" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="C130" s="10" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
     </row>
     <row r="131" spans="1:3" ht="24" customHeight="1">
       <c r="B131" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="132" spans="1:3" ht="178" customHeight="1">
@@ -2691,10 +2701,10 @@
     </row>
     <row r="134" spans="1:3" ht="24" customHeight="1">
       <c r="A134" s="9" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B134" s="9" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
     </row>
     <row r="135" spans="1:3" ht="24" customHeight="1">
@@ -2702,15 +2712,15 @@
         <v>37</v>
       </c>
       <c r="B135" s="10" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="C135" s="10" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="136" spans="1:3" ht="24" customHeight="1">
       <c r="B136" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="137" spans="1:3" ht="178" customHeight="1">
@@ -2718,10 +2728,10 @@
     </row>
     <row r="139" spans="1:3" ht="24" customHeight="1">
       <c r="A139" s="9" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B139" s="9" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row r="140" spans="1:3" ht="24" customHeight="1">
@@ -2729,15 +2739,15 @@
         <v>37</v>
       </c>
       <c r="B140" s="10" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="C140" s="10" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
     </row>
     <row r="141" spans="1:3" ht="24" customHeight="1">
       <c r="B141" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="142" spans="1:3" ht="178" customHeight="1">
@@ -2745,10 +2755,10 @@
     </row>
     <row r="144" spans="1:3" ht="24" customHeight="1">
       <c r="A144" s="9" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B144" s="9" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
     <row r="145" spans="1:3" ht="24" customHeight="1">
@@ -2756,15 +2766,15 @@
         <v>37</v>
       </c>
       <c r="B145" s="10" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C145" s="10" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
     </row>
     <row r="146" spans="1:3" ht="24" customHeight="1">
       <c r="B146" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="147" spans="1:3" ht="178" customHeight="1">
@@ -2772,10 +2782,10 @@
     </row>
     <row r="149" spans="1:3" ht="24" customHeight="1">
       <c r="A149" s="9" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B149" s="9" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="150" spans="1:3" ht="24" customHeight="1">
@@ -2783,15 +2793,15 @@
         <v>37</v>
       </c>
       <c r="B150" s="10" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="C150" s="10" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="151" spans="1:3" ht="24" customHeight="1">
       <c r="B151" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="152" spans="1:3" ht="178" customHeight="1">
@@ -2799,10 +2809,10 @@
     </row>
     <row r="154" spans="1:3" ht="24" customHeight="1">
       <c r="A154" s="9" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B154" s="9" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="155" spans="1:3" ht="24" customHeight="1">
@@ -2810,15 +2820,15 @@
         <v>37</v>
       </c>
       <c r="B155" s="10" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C155" s="10" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
     </row>
     <row r="156" spans="1:3" ht="24" customHeight="1">
       <c r="B156" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="157" spans="1:3" ht="178" customHeight="1">
@@ -2826,23 +2836,23 @@
     </row>
     <row r="160" spans="1:3" ht="24" customHeight="1">
       <c r="A160" s="12" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B160" s="12" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="161" spans="1:3" ht="24" customHeight="1">
       <c r="B161" s="13" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
     </row>
     <row r="163" spans="1:3" ht="24" customHeight="1">
       <c r="A163" s="9" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="B163" s="9" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
     </row>
     <row r="164" spans="1:3" ht="24" customHeight="1">
@@ -2850,15 +2860,15 @@
         <v>37</v>
       </c>
       <c r="B164" s="10" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="C164" s="10" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
     </row>
     <row r="165" spans="1:3" ht="24" customHeight="1">
       <c r="B165" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="166" spans="1:3" ht="178" customHeight="1">
@@ -2866,10 +2876,10 @@
     </row>
     <row r="168" spans="1:3" ht="24" customHeight="1">
       <c r="A168" s="9" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="B168" s="9" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
     </row>
     <row r="169" spans="1:3" ht="24" customHeight="1">
@@ -2877,15 +2887,15 @@
         <v>37</v>
       </c>
       <c r="B169" s="10" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="C169" s="10" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
     </row>
     <row r="170" spans="1:3" ht="24" customHeight="1">
       <c r="B170" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="171" spans="1:3" ht="178" customHeight="1">
@@ -2893,10 +2903,10 @@
     </row>
     <row r="173" spans="1:3" ht="24" customHeight="1">
       <c r="A173" s="9" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="B173" s="9" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row r="174" spans="1:3" ht="24" customHeight="1">
@@ -2904,15 +2914,15 @@
         <v>37</v>
       </c>
       <c r="B174" s="10" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="C174" s="10" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
     </row>
     <row r="175" spans="1:3" ht="24" customHeight="1">
       <c r="B175" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="176" spans="1:3" ht="178" customHeight="1">
@@ -2920,10 +2930,10 @@
     </row>
     <row r="178" spans="1:3" ht="24" customHeight="1">
       <c r="A178" s="9" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="B178" s="9" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
     <row r="179" spans="1:3" ht="24" customHeight="1">
@@ -2931,15 +2941,15 @@
         <v>37</v>
       </c>
       <c r="B179" s="10" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="C179" s="10" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
     <row r="180" spans="1:3" ht="24" customHeight="1">
       <c r="B180" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="181" spans="1:3" ht="178" customHeight="1">
@@ -2947,10 +2957,10 @@
     </row>
     <row r="183" spans="1:3" ht="24" customHeight="1">
       <c r="A183" s="9" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="B183" s="9" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="184" spans="1:3" ht="24" customHeight="1">
@@ -2958,15 +2968,15 @@
         <v>37</v>
       </c>
       <c r="B184" s="10" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="C184" s="10" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
     </row>
     <row r="185" spans="1:3" ht="24" customHeight="1">
       <c r="B185" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="186" spans="1:3" ht="178" customHeight="1">
@@ -2974,10 +2984,10 @@
     </row>
     <row r="188" spans="1:3" ht="24" customHeight="1">
       <c r="A188" s="9" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="B188" s="9" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
     </row>
     <row r="189" spans="1:3" ht="24" customHeight="1">
@@ -2985,15 +2995,15 @@
         <v>37</v>
       </c>
       <c r="B189" s="10" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="C189" s="10" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
     <row r="190" spans="1:3" ht="24" customHeight="1">
       <c r="B190" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="191" spans="1:3" ht="178" customHeight="1">
@@ -3001,10 +3011,10 @@
     </row>
     <row r="193" spans="1:3" ht="24" customHeight="1">
       <c r="A193" s="9" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="B193" s="9" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
     </row>
     <row r="194" spans="1:3" ht="24" customHeight="1">
@@ -3012,15 +3022,15 @@
         <v>37</v>
       </c>
       <c r="B194" s="10" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="C194" s="10" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="195" spans="1:3" ht="24" customHeight="1">
       <c r="B195" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="196" spans="1:3" ht="178" customHeight="1">
@@ -3028,10 +3038,10 @@
     </row>
     <row r="198" spans="1:3" ht="24" customHeight="1">
       <c r="A198" s="9" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="B198" s="9" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
     </row>
     <row r="199" spans="1:3" ht="24" customHeight="1">
@@ -3039,15 +3049,15 @@
         <v>37</v>
       </c>
       <c r="B199" s="10" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="C199" s="10" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
     </row>
     <row r="200" spans="1:3" ht="24" customHeight="1">
       <c r="B200" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="201" spans="1:3" ht="178" customHeight="1">
@@ -3055,10 +3065,10 @@
     </row>
     <row r="203" spans="1:3" ht="24" customHeight="1">
       <c r="A203" s="9" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="B203" s="9" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
     </row>
     <row r="204" spans="1:3" ht="24" customHeight="1">
@@ -3066,15 +3076,15 @@
         <v>37</v>
       </c>
       <c r="B204" s="10" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="C204" s="10" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
     </row>
     <row r="205" spans="1:3" ht="24" customHeight="1">
       <c r="B205" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="206" spans="1:3" ht="178" customHeight="1">
@@ -3082,23 +3092,23 @@
     </row>
     <row r="209" spans="1:3" ht="24" customHeight="1">
       <c r="A209" s="12" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="B209" s="12" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
     </row>
     <row r="210" spans="1:3" ht="24" customHeight="1">
       <c r="B210" s="13" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
     </row>
     <row r="212" spans="1:3" ht="24" customHeight="1">
       <c r="A212" s="9" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="B212" s="9" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="213" spans="1:3" ht="24" customHeight="1">
@@ -3106,15 +3116,15 @@
         <v>37</v>
       </c>
       <c r="B213" s="10" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="C213" s="10" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
     </row>
     <row r="214" spans="1:3" ht="24" customHeight="1">
       <c r="B214" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="215" spans="1:3" ht="178" customHeight="1">
@@ -3122,23 +3132,23 @@
     </row>
     <row r="218" spans="1:3" ht="24" customHeight="1">
       <c r="A218" s="12" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="B218" s="12" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
     </row>
     <row r="219" spans="1:3" ht="24" customHeight="1">
       <c r="B219" s="13" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="221" spans="1:3" ht="24" customHeight="1">
       <c r="A221" s="9" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="B221" s="9" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="222" spans="1:3" ht="24" customHeight="1">
@@ -3146,15 +3156,15 @@
         <v>37</v>
       </c>
       <c r="B222" s="10" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="C222" s="10" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
     </row>
     <row r="223" spans="1:3" ht="24" customHeight="1">
       <c r="B223" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="224" spans="1:3" ht="178" customHeight="1">
@@ -3195,20 +3205,20 @@
   <sheetData>
     <row r="1" spans="1:3" ht="24" customHeight="1">
       <c r="A1" s="12" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="24" customHeight="1">
       <c r="B2" s="13" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="24" customHeight="1">
       <c r="A4" s="9" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>36</v>
@@ -3219,10 +3229,10 @@
         <v>37</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="24" customHeight="1">
@@ -3230,10 +3240,10 @@
     </row>
     <row r="8" spans="1:3" ht="24" customHeight="1">
       <c r="A8" s="9" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="24" customHeight="1">
@@ -3241,15 +3251,15 @@
         <v>37</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="24" customHeight="1">
       <c r="B10" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="178" customHeight="1">
@@ -3257,34 +3267,34 @@
     </row>
     <row r="14" spans="1:3" ht="24" customHeight="1">
       <c r="A14" s="12" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="24" customHeight="1">
       <c r="B15" s="13" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
     </row>
     <row r="17" spans="1:33" ht="24" customHeight="1">
       <c r="A17" s="9" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
     </row>
     <row r="18" spans="1:33" ht="24" customHeight="1">
       <c r="A18" s="14" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
     </row>
     <row r="19" spans="1:33" ht="24" customHeight="1">
@@ -3295,33 +3305,33 @@
     <row r="20" spans="1:33" ht="24" customHeight="1">
       <c r="B20" s="11"/>
       <c r="AA20" s="6" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="AB20" s="6" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="AC20" s="6" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="AD20" s="6" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="AE20" s="6" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="AF20" s="6" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="AG20" s="6" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="22" spans="1:33" ht="24" customHeight="1">
       <c r="A22" s="9" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
     <row r="23" spans="1:33" ht="24" customHeight="1">
@@ -3329,15 +3339,15 @@
         <v>37</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
     </row>
     <row r="24" spans="1:33" ht="24" customHeight="1">
       <c r="B24" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="25" spans="1:33" ht="178" customHeight="1">
@@ -3345,34 +3355,34 @@
     </row>
     <row r="28" spans="1:33" ht="24" customHeight="1">
       <c r="A28" s="12" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
     </row>
     <row r="29" spans="1:33" ht="24" customHeight="1">
       <c r="B29" s="13" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
     </row>
     <row r="31" spans="1:33" ht="24" customHeight="1">
       <c r="A31" s="9" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
     </row>
     <row r="32" spans="1:33" ht="24" customHeight="1">
       <c r="A32" s="14" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
     </row>
     <row r="33" spans="1:33" ht="24" customHeight="1">
@@ -3383,33 +3393,33 @@
     <row r="34" spans="1:33" ht="24" customHeight="1">
       <c r="B34" s="11"/>
       <c r="AA34" s="6" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="AB34" s="6" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="AC34" s="6" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="AD34" s="6" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="AE34" s="6" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="AF34" s="6" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="AG34" s="6" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="36" spans="1:33" ht="24" customHeight="1">
       <c r="A36" s="9" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
     <row r="37" spans="1:33" ht="24" customHeight="1">
@@ -3417,15 +3427,15 @@
         <v>37</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="C37" s="10" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
     </row>
     <row r="38" spans="1:33" ht="24" customHeight="1">
       <c r="B38" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="39" spans="1:33" ht="178" customHeight="1">
@@ -3433,34 +3443,34 @@
     </row>
     <row r="42" spans="1:33" ht="24" customHeight="1">
       <c r="A42" s="12" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="B42" s="12" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
     </row>
     <row r="43" spans="1:33" ht="24" customHeight="1">
       <c r="B43" s="13" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
     </row>
     <row r="45" spans="1:33" ht="24" customHeight="1">
       <c r="A45" s="9" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
     </row>
     <row r="46" spans="1:33" ht="24" customHeight="1">
       <c r="A46" s="14" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="C46" s="10" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
     </row>
     <row r="47" spans="1:33" ht="24" customHeight="1">
@@ -3471,33 +3481,33 @@
     <row r="48" spans="1:33" ht="24" customHeight="1">
       <c r="B48" s="11"/>
       <c r="AA48" s="6" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="AB48" s="6" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="AC48" s="6" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="AD48" s="6" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="AE48" s="6" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="AF48" s="6" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="AG48" s="6" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="50" spans="1:33" ht="24" customHeight="1">
       <c r="A50" s="9" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
     <row r="51" spans="1:33" ht="24" customHeight="1">
@@ -3505,15 +3515,15 @@
         <v>37</v>
       </c>
       <c r="B51" s="10" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="C51" s="10" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
     </row>
     <row r="52" spans="1:33" ht="24" customHeight="1">
       <c r="B52" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="53" spans="1:33" ht="178" customHeight="1">
@@ -3521,34 +3531,34 @@
     </row>
     <row r="56" spans="1:33" ht="24" customHeight="1">
       <c r="A56" s="12" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="B56" s="12" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
     </row>
     <row r="57" spans="1:33" ht="24" customHeight="1">
       <c r="B57" s="13" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
     </row>
     <row r="59" spans="1:33" ht="24" customHeight="1">
       <c r="A59" s="9" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
     </row>
     <row r="60" spans="1:33" ht="24" customHeight="1">
       <c r="A60" s="14" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B60" s="10" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="C60" s="10" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
     </row>
     <row r="61" spans="1:33" ht="24" customHeight="1">
@@ -3559,33 +3569,33 @@
     <row r="62" spans="1:33" ht="24" customHeight="1">
       <c r="B62" s="11"/>
       <c r="AA62" s="6" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="AB62" s="6" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="AC62" s="6" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="AD62" s="6" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="AE62" s="6" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="AF62" s="6" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="AG62" s="6" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="64" spans="1:33" ht="24" customHeight="1">
       <c r="A64" s="9" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="B64" s="9" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
     <row r="65" spans="1:33" ht="24" customHeight="1">
@@ -3593,15 +3603,15 @@
         <v>37</v>
       </c>
       <c r="B65" s="10" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="C65" s="10" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
     </row>
     <row r="66" spans="1:33" ht="24" customHeight="1">
       <c r="B66" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="67" spans="1:33" ht="178" customHeight="1">
@@ -3609,34 +3619,34 @@
     </row>
     <row r="70" spans="1:33" ht="24" customHeight="1">
       <c r="A70" s="12" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="B70" s="12" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
     </row>
     <row r="71" spans="1:33" ht="24" customHeight="1">
       <c r="B71" s="13" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
     </row>
     <row r="73" spans="1:33" ht="24" customHeight="1">
       <c r="A73" s="9" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="B73" s="9" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
     </row>
     <row r="74" spans="1:33" ht="24" customHeight="1">
       <c r="A74" s="14" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B74" s="10" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="C74" s="10" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
     </row>
     <row r="75" spans="1:33" ht="24" customHeight="1">
@@ -3647,33 +3657,33 @@
     <row r="76" spans="1:33" ht="24" customHeight="1">
       <c r="B76" s="11"/>
       <c r="AA76" s="6" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="AB76" s="6" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="AC76" s="6" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="AD76" s="6" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="AE76" s="6" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="AF76" s="6" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="AG76" s="6" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="78" spans="1:33" ht="24" customHeight="1">
       <c r="A78" s="9" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="B78" s="9" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
     <row r="79" spans="1:33" ht="24" customHeight="1">
@@ -3681,15 +3691,15 @@
         <v>37</v>
       </c>
       <c r="B79" s="10" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="C79" s="10" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
     </row>
     <row r="80" spans="1:33" ht="24" customHeight="1">
       <c r="B80" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="81" spans="1:33" ht="178" customHeight="1">
@@ -3697,34 +3707,34 @@
     </row>
     <row r="84" spans="1:33" ht="24" customHeight="1">
       <c r="A84" s="12" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="B84" s="12" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
     </row>
     <row r="85" spans="1:33" ht="24" customHeight="1">
       <c r="B85" s="13" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
     </row>
     <row r="87" spans="1:33" ht="24" customHeight="1">
       <c r="A87" s="9" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="B87" s="9" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
     </row>
     <row r="88" spans="1:33" ht="24" customHeight="1">
       <c r="A88" s="14" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B88" s="10" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="C88" s="10" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
     </row>
     <row r="89" spans="1:33" ht="24" customHeight="1">
@@ -3735,70 +3745,70 @@
     <row r="90" spans="1:33" ht="24" customHeight="1">
       <c r="B90" s="11"/>
       <c r="AA90" s="6" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="AB90" s="6" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="AC90" s="6" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="AD90" s="6" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="AE90" s="6" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="AF90" s="6" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="AG90" s="6" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="92" spans="1:33" ht="24" customHeight="1">
       <c r="A92" s="9" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="B92" s="9" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
     </row>
     <row r="93" spans="1:33" ht="24" customHeight="1">
       <c r="A93" s="14" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B93" s="10" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="C93" s="10" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
     </row>
     <row r="94" spans="1:33" ht="24" customHeight="1">
       <c r="B94" s="11"/>
       <c r="AA94" s="6" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="AB94" s="6" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="AC94" s="6" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="AD94" s="6" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="AE94" s="6" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="96" spans="1:33" ht="24" customHeight="1">
       <c r="A96" s="9" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="B96" s="9" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
     <row r="97" spans="1:33" ht="24" customHeight="1">
@@ -3806,15 +3816,15 @@
         <v>37</v>
       </c>
       <c r="B97" s="10" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="C97" s="10" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
     </row>
     <row r="98" spans="1:33" ht="24" customHeight="1">
       <c r="B98" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="99" spans="1:33" ht="178" customHeight="1">
@@ -3822,34 +3832,34 @@
     </row>
     <row r="102" spans="1:33" ht="24" customHeight="1">
       <c r="A102" s="12" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="B102" s="12" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
     </row>
     <row r="103" spans="1:33" ht="24" customHeight="1">
       <c r="B103" s="13" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
     </row>
     <row r="105" spans="1:33" ht="24" customHeight="1">
       <c r="A105" s="9" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="B105" s="9" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
     </row>
     <row r="106" spans="1:33" ht="24" customHeight="1">
       <c r="A106" s="14" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B106" s="10" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="C106" s="10" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="107" spans="1:33" ht="24" customHeight="1">
@@ -3860,33 +3870,33 @@
     <row r="108" spans="1:33" ht="24" customHeight="1">
       <c r="B108" s="11"/>
       <c r="AA108" s="6" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="AB108" s="6" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="AC108" s="6" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="AD108" s="6" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="AE108" s="6" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="AF108" s="6" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="AG108" s="6" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="110" spans="1:33" ht="24" customHeight="1">
       <c r="A110" s="9" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="B110" s="9" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
     <row r="111" spans="1:33" ht="24" customHeight="1">
@@ -3894,15 +3904,15 @@
         <v>37</v>
       </c>
       <c r="B111" s="10" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="C111" s="10" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
     </row>
     <row r="112" spans="1:33" ht="24" customHeight="1">
       <c r="B112" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="113" spans="1:33" ht="178" customHeight="1">
@@ -3910,34 +3920,34 @@
     </row>
     <row r="116" spans="1:33" ht="24" customHeight="1">
       <c r="A116" s="12" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="B116" s="12" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
     </row>
     <row r="117" spans="1:33" ht="24" customHeight="1">
       <c r="B117" s="13" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
     </row>
     <row r="119" spans="1:33" ht="24" customHeight="1">
       <c r="A119" s="9" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="B119" s="9" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
     </row>
     <row r="120" spans="1:33" ht="24" customHeight="1">
       <c r="A120" s="14" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B120" s="10" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="C120" s="10" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
     </row>
     <row r="121" spans="1:33" ht="24" customHeight="1">
@@ -3948,33 +3958,33 @@
     <row r="122" spans="1:33" ht="24" customHeight="1">
       <c r="B122" s="11"/>
       <c r="AA122" s="6" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="AB122" s="6" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="AC122" s="6" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="AD122" s="6" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="AE122" s="6" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="AF122" s="6" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="AG122" s="6" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="124" spans="1:33" ht="24" customHeight="1">
       <c r="A124" s="9" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="B124" s="9" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
     <row r="125" spans="1:33" ht="24" customHeight="1">
@@ -3982,15 +3992,15 @@
         <v>37</v>
       </c>
       <c r="B125" s="10" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="C125" s="10" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
     </row>
     <row r="126" spans="1:33" ht="24" customHeight="1">
       <c r="B126" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="127" spans="1:33" ht="178" customHeight="1">
@@ -3998,34 +4008,34 @@
     </row>
     <row r="130" spans="1:33" ht="24" customHeight="1">
       <c r="A130" s="12" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="B130" s="12" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
     </row>
     <row r="131" spans="1:33" ht="24" customHeight="1">
       <c r="B131" s="13" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
     </row>
     <row r="133" spans="1:33" ht="24" customHeight="1">
       <c r="A133" s="9" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="B133" s="9" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
     </row>
     <row r="134" spans="1:33" ht="24" customHeight="1">
       <c r="A134" s="14" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B134" s="10" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="C134" s="10" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
     </row>
     <row r="135" spans="1:33" ht="24" customHeight="1">
@@ -4036,33 +4046,33 @@
     <row r="136" spans="1:33" ht="24" customHeight="1">
       <c r="B136" s="11"/>
       <c r="AA136" s="6" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="AB136" s="6" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="AC136" s="6" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="AD136" s="6" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="AE136" s="6" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="AF136" s="6" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="AG136" s="6" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="138" spans="1:33" ht="24" customHeight="1">
       <c r="A138" s="9" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="B138" s="9" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
     <row r="139" spans="1:33" ht="24" customHeight="1">
@@ -4070,15 +4080,15 @@
         <v>37</v>
       </c>
       <c r="B139" s="10" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="C139" s="10" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
     </row>
     <row r="140" spans="1:33" ht="24" customHeight="1">
       <c r="B140" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="141" spans="1:33" ht="178" customHeight="1">
@@ -4086,34 +4096,34 @@
     </row>
     <row r="144" spans="1:33" ht="24" customHeight="1">
       <c r="A144" s="12" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="B144" s="12" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
     </row>
     <row r="145" spans="1:33" ht="24" customHeight="1">
       <c r="B145" s="13" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
     </row>
     <row r="147" spans="1:33" ht="24" customHeight="1">
       <c r="A147" s="9" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="B147" s="9" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
     </row>
     <row r="148" spans="1:33" ht="24" customHeight="1">
       <c r="A148" s="14" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B148" s="10" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="C148" s="10" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
     </row>
     <row r="149" spans="1:33" ht="24" customHeight="1">
@@ -4124,33 +4134,33 @@
     <row r="150" spans="1:33" ht="24" customHeight="1">
       <c r="B150" s="11"/>
       <c r="AA150" s="6" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="AB150" s="6" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="AC150" s="6" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="AD150" s="6" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="AE150" s="6" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="AF150" s="6" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="AG150" s="6" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="152" spans="1:33" ht="24" customHeight="1">
       <c r="A152" s="9" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="B152" s="9" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
     <row r="153" spans="1:33" ht="24" customHeight="1">
@@ -4158,15 +4168,15 @@
         <v>37</v>
       </c>
       <c r="B153" s="10" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="C153" s="10" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
     </row>
     <row r="154" spans="1:33" ht="24" customHeight="1">
       <c r="B154" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="155" spans="1:33" ht="178" customHeight="1">
@@ -4174,34 +4184,34 @@
     </row>
     <row r="158" spans="1:33" ht="24" customHeight="1">
       <c r="A158" s="12" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="B158" s="12" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
     </row>
     <row r="159" spans="1:33" ht="24" customHeight="1">
       <c r="B159" s="13" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
     </row>
     <row r="161" spans="1:33" ht="24" customHeight="1">
       <c r="A161" s="9" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="B161" s="9" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
     </row>
     <row r="162" spans="1:33" ht="24" customHeight="1">
       <c r="A162" s="14" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B162" s="10" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="C162" s="10" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
     </row>
     <row r="163" spans="1:33" ht="24" customHeight="1">
@@ -4212,44 +4222,44 @@
     <row r="164" spans="1:33" ht="24" customHeight="1">
       <c r="B164" s="11"/>
       <c r="AA164" s="6" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="AB164" s="6" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="AC164" s="6" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="AD164" s="6" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="AE164" s="6" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="AF164" s="6" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="AG164" s="6" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="166" spans="1:33" ht="24" customHeight="1">
       <c r="A166" s="9" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="B166" s="9" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
     </row>
     <row r="167" spans="1:33" ht="24" customHeight="1">
       <c r="A167" s="14" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B167" s="10" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="C167" s="10" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
     </row>
     <row r="168" spans="1:33" ht="24" customHeight="1">
@@ -4257,10 +4267,10 @@
     </row>
     <row r="170" spans="1:33" ht="24" customHeight="1">
       <c r="A170" s="9" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="B170" s="9" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
     <row r="171" spans="1:33" ht="24" customHeight="1">
@@ -4268,15 +4278,15 @@
         <v>37</v>
       </c>
       <c r="B171" s="10" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="C171" s="10" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
     </row>
     <row r="172" spans="1:33" ht="24" customHeight="1">
       <c r="B172" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="173" spans="1:33" ht="178" customHeight="1">
@@ -4284,34 +4294,34 @@
     </row>
     <row r="176" spans="1:33" ht="24" customHeight="1">
       <c r="A176" s="12" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="B176" s="12" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
     </row>
     <row r="177" spans="1:33" ht="24" customHeight="1">
       <c r="B177" s="13" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
     </row>
     <row r="179" spans="1:33" ht="24" customHeight="1">
       <c r="A179" s="9" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="B179" s="9" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
     </row>
     <row r="180" spans="1:33" ht="24" customHeight="1">
       <c r="A180" s="14" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B180" s="10" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="C180" s="10" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
     </row>
     <row r="181" spans="1:33" ht="24" customHeight="1">
@@ -4322,44 +4332,44 @@
     <row r="182" spans="1:33" ht="24" customHeight="1">
       <c r="B182" s="11"/>
       <c r="AA182" s="6" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="AB182" s="6" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="AC182" s="6" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="AD182" s="6" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="AE182" s="6" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="AF182" s="6" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="AG182" s="6" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="184" spans="1:33" ht="24" customHeight="1">
       <c r="A184" s="9" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="B184" s="9" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
     </row>
     <row r="185" spans="1:33" ht="24" customHeight="1">
       <c r="A185" s="14" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B185" s="10" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="C185" s="10" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
     </row>
     <row r="186" spans="1:33" ht="24" customHeight="1">
@@ -4367,21 +4377,21 @@
     </row>
     <row r="188" spans="1:33" ht="24" customHeight="1">
       <c r="A188" s="9" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="B188" s="9" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
     </row>
     <row r="189" spans="1:33" ht="24" customHeight="1">
       <c r="A189" s="14" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B189" s="10" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="C189" s="10" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
     </row>
     <row r="190" spans="1:33" ht="24" customHeight="1">
@@ -4389,10 +4399,10 @@
     </row>
     <row r="192" spans="1:33" ht="24" customHeight="1">
       <c r="A192" s="9" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="B192" s="9" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
     <row r="193" spans="1:33" ht="24" customHeight="1">
@@ -4400,15 +4410,15 @@
         <v>37</v>
       </c>
       <c r="B193" s="10" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="C193" s="10" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
     </row>
     <row r="194" spans="1:33" ht="24" customHeight="1">
       <c r="B194" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="195" spans="1:33" ht="178" customHeight="1">
@@ -4416,34 +4426,34 @@
     </row>
     <row r="198" spans="1:33" ht="24" customHeight="1">
       <c r="A198" s="12" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="B198" s="12" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
     </row>
     <row r="199" spans="1:33" ht="24" customHeight="1">
       <c r="B199" s="13" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
     </row>
     <row r="201" spans="1:33" ht="24" customHeight="1">
       <c r="A201" s="9" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="B201" s="9" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
     </row>
     <row r="202" spans="1:33" ht="24" customHeight="1">
       <c r="A202" s="14" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B202" s="10" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="C202" s="10" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
     </row>
     <row r="203" spans="1:33" ht="24" customHeight="1">
@@ -4454,33 +4464,33 @@
     <row r="204" spans="1:33" ht="24" customHeight="1">
       <c r="B204" s="11"/>
       <c r="AA204" s="6" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="AB204" s="6" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="AC204" s="6" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="AD204" s="6" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="AE204" s="6" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="AF204" s="6" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="AG204" s="6" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="206" spans="1:33" ht="24" customHeight="1">
       <c r="A206" s="9" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="B206" s="9" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
     <row r="207" spans="1:33" ht="24" customHeight="1">
@@ -4488,15 +4498,15 @@
         <v>37</v>
       </c>
       <c r="B207" s="10" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="C207" s="10" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
     </row>
     <row r="208" spans="1:33" ht="24" customHeight="1">
       <c r="B208" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="209" spans="1:33" ht="178" customHeight="1">
@@ -4504,34 +4514,34 @@
     </row>
     <row r="212" spans="1:33" ht="24" customHeight="1">
       <c r="A212" s="12" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="B212" s="12" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
     </row>
     <row r="213" spans="1:33" ht="24" customHeight="1">
       <c r="B213" s="13" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
     </row>
     <row r="215" spans="1:33" ht="24" customHeight="1">
       <c r="A215" s="9" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="B215" s="9" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
     </row>
     <row r="216" spans="1:33" ht="24" customHeight="1">
       <c r="A216" s="14" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B216" s="10" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="C216" s="10" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
     </row>
     <row r="217" spans="1:33" ht="24" customHeight="1">
@@ -4542,113 +4552,113 @@
     <row r="218" spans="1:33" ht="24" customHeight="1">
       <c r="B218" s="11"/>
       <c r="AA218" s="6" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="AB218" s="6" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="AC218" s="6" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="AD218" s="6" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="AE218" s="6" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="AF218" s="6" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="AG218" s="6" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="220" spans="1:33" ht="24" customHeight="1">
       <c r="A220" s="9" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="B220" s="9" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
     </row>
     <row r="221" spans="1:33" ht="24" customHeight="1">
       <c r="A221" s="14" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B221" s="10" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="C221" s="10" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
     </row>
     <row r="222" spans="1:33" ht="24" customHeight="1">
       <c r="B222" s="11"/>
       <c r="AA222" s="6" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="AB222" s="6" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="AC222" s="6" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="AD222" s="6" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="AE222" s="6" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="AF222" s="6" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="224" spans="1:33" ht="24" customHeight="1">
       <c r="A224" s="9" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="B224" s="9" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
     </row>
     <row r="225" spans="1:33" ht="24" customHeight="1">
       <c r="A225" s="14" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B225" s="10" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="C225" s="10" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
     </row>
     <row r="226" spans="1:33" ht="24" customHeight="1">
       <c r="B226" s="11"/>
       <c r="AA226" s="6" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="AB226" s="6" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="AC226" s="6" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="AD226" s="6" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="AE226" s="6" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="AF226" s="6" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="228" spans="1:33" ht="24" customHeight="1">
       <c r="A228" s="9" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="B228" s="9" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
     <row r="229" spans="1:33" ht="24" customHeight="1">
@@ -4656,15 +4666,15 @@
         <v>37</v>
       </c>
       <c r="B229" s="10" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="C229" s="10" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
     </row>
     <row r="230" spans="1:33" ht="24" customHeight="1">
       <c r="B230" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="231" spans="1:33" ht="178" customHeight="1">
@@ -4672,34 +4682,34 @@
     </row>
     <row r="234" spans="1:33" ht="24" customHeight="1">
       <c r="A234" s="12" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="B234" s="12" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
     </row>
     <row r="235" spans="1:33" ht="24" customHeight="1">
       <c r="B235" s="13" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
     </row>
     <row r="237" spans="1:33" ht="24" customHeight="1">
       <c r="A237" s="9" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="B237" s="9" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
     </row>
     <row r="238" spans="1:33" ht="24" customHeight="1">
       <c r="A238" s="14" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B238" s="10" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="C238" s="10" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
     </row>
     <row r="239" spans="1:33" ht="24" customHeight="1">
@@ -4710,113 +4720,113 @@
     <row r="240" spans="1:33" ht="24" customHeight="1">
       <c r="B240" s="11"/>
       <c r="AA240" s="6" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="AB240" s="6" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="AC240" s="6" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="AD240" s="6" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="AE240" s="6" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="AF240" s="6" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="AG240" s="6" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="242" spans="1:32" ht="24" customHeight="1">
       <c r="A242" s="9" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="B242" s="9" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
     </row>
     <row r="243" spans="1:32" ht="24" customHeight="1">
       <c r="A243" s="14" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B243" s="10" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="C243" s="10" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
     </row>
     <row r="244" spans="1:32" ht="24" customHeight="1">
       <c r="B244" s="11"/>
       <c r="AA244" s="6" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="AB244" s="6" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="AC244" s="6" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="AD244" s="6" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="AE244" s="6" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="AF244" s="6" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="246" spans="1:32" ht="24" customHeight="1">
       <c r="A246" s="9" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="B246" s="9" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
     </row>
     <row r="247" spans="1:32" ht="24" customHeight="1">
       <c r="A247" s="14" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B247" s="10" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="C247" s="10" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
     </row>
     <row r="248" spans="1:32" ht="24" customHeight="1">
       <c r="B248" s="11"/>
       <c r="AA248" s="6" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="AB248" s="6" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="AC248" s="6" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="AD248" s="6" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="AE248" s="6" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="AF248" s="6" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="250" spans="1:32" ht="24" customHeight="1">
       <c r="A250" s="9" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="B250" s="9" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
     <row r="251" spans="1:32" ht="24" customHeight="1">
@@ -4824,15 +4834,15 @@
         <v>37</v>
       </c>
       <c r="B251" s="10" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="C251" s="10" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
     </row>
     <row r="252" spans="1:32" ht="24" customHeight="1">
       <c r="B252" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="253" spans="1:32" ht="178" customHeight="1">
@@ -4840,34 +4850,34 @@
     </row>
     <row r="256" spans="1:32" ht="24" customHeight="1">
       <c r="A256" s="12" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="B256" s="12" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
     </row>
     <row r="257" spans="1:33" ht="24" customHeight="1">
       <c r="B257" s="13" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
     </row>
     <row r="259" spans="1:33" ht="24" customHeight="1">
       <c r="A259" s="9" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="B259" s="9" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
     </row>
     <row r="260" spans="1:33" ht="24" customHeight="1">
       <c r="A260" s="14" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B260" s="10" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="C260" s="10" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
     </row>
     <row r="261" spans="1:33" ht="24" customHeight="1">
@@ -4878,33 +4888,33 @@
     <row r="262" spans="1:33" ht="24" customHeight="1">
       <c r="B262" s="11"/>
       <c r="AA262" s="6" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="AB262" s="6" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="AC262" s="6" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="AD262" s="6" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="AE262" s="6" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="AF262" s="6" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="AG262" s="6" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="264" spans="1:33" ht="24" customHeight="1">
       <c r="A264" s="9" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="B264" s="9" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
     <row r="265" spans="1:33" ht="24" customHeight="1">
@@ -4912,15 +4922,15 @@
         <v>37</v>
       </c>
       <c r="B265" s="10" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="C265" s="10" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
     </row>
     <row r="266" spans="1:33" ht="24" customHeight="1">
       <c r="B266" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="267" spans="1:33" ht="178" customHeight="1">
@@ -4928,34 +4938,34 @@
     </row>
     <row r="270" spans="1:33" ht="24" customHeight="1">
       <c r="A270" s="12" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="B270" s="12" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
     </row>
     <row r="271" spans="1:33" ht="24" customHeight="1">
       <c r="B271" s="13" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
     </row>
     <row r="273" spans="1:33" ht="24" customHeight="1">
       <c r="A273" s="9" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="B273" s="9" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
     </row>
     <row r="274" spans="1:33" ht="24" customHeight="1">
       <c r="A274" s="14" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B274" s="10" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="C274" s="10" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
     </row>
     <row r="275" spans="1:33" ht="24" customHeight="1">
@@ -4966,44 +4976,44 @@
     <row r="276" spans="1:33" ht="24" customHeight="1">
       <c r="B276" s="11"/>
       <c r="AA276" s="6" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="AB276" s="6" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="AC276" s="6" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="AD276" s="6" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="AE276" s="6" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="AF276" s="6" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="AG276" s="6" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="278" spans="1:33" ht="24" customHeight="1">
       <c r="A278" s="9" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="B278" s="9" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
     </row>
     <row r="279" spans="1:33" ht="24" customHeight="1">
       <c r="A279" s="14" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B279" s="10" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="C279" s="10" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
     </row>
     <row r="280" spans="1:33" ht="24" customHeight="1">
@@ -5011,10 +5021,10 @@
     </row>
     <row r="282" spans="1:33" ht="24" customHeight="1">
       <c r="A282" s="9" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="B282" s="9" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
     <row r="283" spans="1:33" ht="24" customHeight="1">
@@ -5022,15 +5032,15 @@
         <v>37</v>
       </c>
       <c r="B283" s="10" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="C283" s="10" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
     </row>
     <row r="284" spans="1:33" ht="24" customHeight="1">
       <c r="B284" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="285" spans="1:33" ht="178" customHeight="1">
@@ -5038,34 +5048,34 @@
     </row>
     <row r="288" spans="1:33" ht="24" customHeight="1">
       <c r="A288" s="12" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="B288" s="12" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
     </row>
     <row r="289" spans="1:32" ht="24" customHeight="1">
       <c r="B289" s="13" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
     </row>
     <row r="291" spans="1:32" ht="24" customHeight="1">
       <c r="A291" s="9" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="B291" s="9" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
     </row>
     <row r="292" spans="1:32" ht="24" customHeight="1">
       <c r="A292" s="14" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B292" s="10" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="C292" s="10" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
     </row>
     <row r="293" spans="1:32" ht="24" customHeight="1">
@@ -5076,30 +5086,30 @@
     <row r="294" spans="1:32" ht="24" customHeight="1">
       <c r="B294" s="11"/>
       <c r="AA294" s="6" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="AB294" s="6" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="AC294" s="6" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="AD294" s="6" t="s">
-        <v>414</v>
+        <v>416</v>
       </c>
       <c r="AE294" s="6" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="AF294" s="6" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="296" spans="1:32" ht="24" customHeight="1">
       <c r="A296" s="9" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="B296" s="9" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
     <row r="297" spans="1:32" ht="24" customHeight="1">
@@ -5107,15 +5117,15 @@
         <v>37</v>
       </c>
       <c r="B297" s="10" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="C297" s="10" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
     </row>
     <row r="298" spans="1:32" ht="24" customHeight="1">
       <c r="B298" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="299" spans="1:32" ht="178" customHeight="1">

</xml_diff>